<commit_message>
added mcnemar for cluster methods, k fold accuracy
</commit_message>
<xml_diff>
--- a/model_metrics.xlsx
+++ b/model_metrics.xlsx
@@ -24,24 +24,24 @@
     <t>Random Forest</t>
   </si>
   <si>
-    <t>K-Nearest Neighbors</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
     <t>McNemar vs LogReg</t>
   </si>
   <si>
     <t>Neural Network</t>
   </si>
+  <si>
+    <t>Accuracy (Over 4 Folds)</t>
+  </si>
+  <si>
+    <t>Cluster</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -87,7 +87,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,18 +392,18 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:E9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="22.26953125" style="1" customWidth="1"/>
+    <col min="1" max="5" width="19.54296875" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -425,63 +425,63 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.95189999999999997</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.67025462962962901</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.59519999999999995</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.50970000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.93942901234567899</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.75833333333333297</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.56777777777777705</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.52426697530864197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.93603395061728401</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.67025462962962901</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.52449074074073998</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.51018518518518496</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1">
-        <v>18</v>
+        <v>3</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -490,15 +490,15 @@
         <v>0</v>
       </c>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>0.214</v>
       </c>
       <c r="E8" s="3">
-        <v>0</v>
+        <v>0.96899999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -507,10 +507,10 @@
         <v>0</v>
       </c>
       <c r="D9" s="3">
-        <v>0.214</v>
+        <v>0.50248165485657903</v>
       </c>
       <c r="E9" s="3">
-        <v>0.96899999999999997</v>
+        <v>0.43824309778037002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tidy up code for train test split, random forest
</commit_message>
<xml_diff>
--- a/model_metrics.xlsx
+++ b/model_metrics.xlsx
@@ -391,13 +391,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="19.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7265625" style="1" customWidth="1"/>
+    <col min="2" max="5" width="8.7265625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
@@ -431,7 +432,7 @@
         <v>0.95189999999999997</v>
       </c>
       <c r="C3" s="3">
-        <v>0.67025462962962901</v>
+        <v>0.86580000000000001</v>
       </c>
       <c r="D3" s="3">
         <v>0.59519999999999995</v>
@@ -490,10 +491,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="3">
-        <v>0.214</v>
+        <v>0.22106191159593699</v>
       </c>
       <c r="E8" s="3">
-        <v>0.96899999999999997</v>
+        <v>0.984708287874275</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -504,13 +505,13 @@
         <v>0</v>
       </c>
       <c r="C9" s="3">
-        <v>0</v>
+        <v>6.0524851590652497E-13</v>
       </c>
       <c r="D9" s="3">
-        <v>0.50248165485657903</v>
+        <v>0.49043076211320802</v>
       </c>
       <c r="E9" s="3">
-        <v>0.43824309778037002</v>
+        <v>0.44895933125744703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added docstrings to most important functions
</commit_message>
<xml_diff>
--- a/model_metrics.xlsx
+++ b/model_metrics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>n</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>Cluster</t>
+  </si>
+  <si>
+    <t>Precision (Over 4 Folds)</t>
+  </si>
+  <si>
+    <t>Recall (Over 4 Folds)</t>
+  </si>
+  <si>
+    <t>F1 (Over 4 Folds)</t>
   </si>
 </sst>
 </file>
@@ -389,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -443,7 +452,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -465,52 +474,187 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.86609999999999998</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.59519999999999995</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.50990000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.95189999999999997</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.86580000000000001</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.59619999999999995</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.50970000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1">
+        <v>15</v>
+      </c>
+      <c r="E14" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.95189999999999997</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.86580000000000001</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.5948</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.50939999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1">
+        <v>12</v>
+      </c>
+      <c r="D18" s="1">
+        <v>15</v>
+      </c>
+      <c r="E18" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
         <v>0.22106191159593699</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E20" s="3">
         <v>0.984708287874275</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3">
         <v>6.0524851590652497E-13</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D21" s="3">
         <v>0.49043076211320802</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E21" s="3">
         <v>0.44895933125744703</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rename files for clarity
</commit_message>
<xml_diff>
--- a/model_metrics.xlsx
+++ b/model_metrics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>n</t>
   </si>
@@ -43,6 +43,54 @@
   </si>
   <si>
     <t>F1 (Over 4 Folds)</t>
+  </si>
+  <si>
+    <t>RF Hyperparameters</t>
+  </si>
+  <si>
+    <t>n_estimators</t>
+  </si>
+  <si>
+    <t>max_depth</t>
+  </si>
+  <si>
+    <t>min_samples_split</t>
+  </si>
+  <si>
+    <t>min_samples_leaf</t>
+  </si>
+  <si>
+    <t>max_features</t>
+  </si>
+  <si>
+    <t>log2</t>
+  </si>
+  <si>
+    <t>sqrt</t>
+  </si>
+  <si>
+    <t>n_components</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>number of trees per forest</t>
+  </si>
+  <si>
+    <t>maximum depth of each tree</t>
+  </si>
+  <si>
+    <t>minimum number of samples for each split</t>
+  </si>
+  <si>
+    <t>minimum number of samples for each leaf node</t>
+  </si>
+  <si>
+    <t>maximum number of features in each tree</t>
+  </si>
+  <si>
+    <t>number of PCA components</t>
   </si>
 </sst>
 </file>
@@ -92,11 +140,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,17 +449,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.7265625" style="1" customWidth="1"/>
     <col min="2" max="5" width="8.7265625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="28.1796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -585,12 +637,12 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -624,7 +676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -641,7 +693,7 @@
         <v>0.984708287874275</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -656,6 +708,151 @@
       </c>
       <c r="E21" s="3">
         <v>0.44895933125744703</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1">
+        <v>9</v>
+      </c>
+      <c r="C24" s="1">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1">
+        <v>15</v>
+      </c>
+      <c r="E24" s="1">
+        <v>18</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1">
+        <v>500</v>
+      </c>
+      <c r="C25" s="1">
+        <v>500</v>
+      </c>
+      <c r="D25" s="1">
+        <v>500</v>
+      </c>
+      <c r="E25" s="1">
+        <v>500</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="1">
+        <v>20</v>
+      </c>
+      <c r="C26" s="1">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1">
+        <v>29</v>
+      </c>
+      <c r="E26" s="1">
+        <v>17</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1">
+        <v>14</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>17</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1">
+        <v>4</v>
+      </c>
+      <c r="E30" s="1">
+        <v>15</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>